<commit_message>
Rows and columns complete
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="10545"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stage 0" sheetId="1" r:id="rId1"/>
@@ -16,32 +16,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>PC1</t>
-  </si>
-  <si>
-    <t>PC0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="123">
   <si>
     <t>PC</t>
   </si>
   <si>
-    <t>IR1_1</t>
-  </si>
-  <si>
-    <t>IR0_1</t>
-  </si>
-  <si>
     <t>IR_1</t>
   </si>
   <si>
     <t>PCs_en</t>
   </si>
   <si>
-    <t>PCs_C</t>
-  </si>
-  <si>
     <t>PC Stack</t>
   </si>
   <si>
@@ -109,6 +94,297 @@
   </si>
   <si>
     <t>set</t>
+  </si>
+  <si>
+    <t>Mar_s</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>MUX_MAR</t>
+  </si>
+  <si>
+    <t>CP9</t>
+  </si>
+  <si>
+    <t>B_MUX</t>
+  </si>
+  <si>
+    <t>CP11</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B_s</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A_s</t>
+  </si>
+  <si>
+    <t>A_MUX</t>
+  </si>
+  <si>
+    <t>CP10</t>
+  </si>
+  <si>
+    <t>CCR</t>
+  </si>
+  <si>
+    <t>CCR_s</t>
+  </si>
+  <si>
+    <t>MUX_ALU</t>
+  </si>
+  <si>
+    <t>CP1</t>
+  </si>
+  <si>
+    <t>CP0</t>
+  </si>
+  <si>
+    <t>Alu_ctrl[0]</t>
+  </si>
+  <si>
+    <t>Alu_ctrl[1]</t>
+  </si>
+  <si>
+    <t>Alu_ctrl[2]</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>ACC_s</t>
+  </si>
+  <si>
+    <t>Shifter</t>
+  </si>
+  <si>
+    <t>Sh_ctrl[0]</t>
+  </si>
+  <si>
+    <t>Sh_ctrl[1]</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>num_shift</t>
+  </si>
+  <si>
+    <t>Accum Stack</t>
+  </si>
+  <si>
+    <t>ACCs_en</t>
+  </si>
+  <si>
+    <t>ACCs_ctrl</t>
+  </si>
+  <si>
+    <t>MUX_ACC</t>
+  </si>
+  <si>
+    <t>CP5</t>
+  </si>
+  <si>
+    <t>CP6</t>
+  </si>
+  <si>
+    <t>CP2</t>
+  </si>
+  <si>
+    <t>CP3</t>
+  </si>
+  <si>
+    <t>CP4</t>
+  </si>
+  <si>
+    <t>MUX_MDR</t>
+  </si>
+  <si>
+    <t>MDR</t>
+  </si>
+  <si>
+    <t>Mdr_s</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>CH_HIT</t>
+  </si>
+  <si>
+    <t>CH_en</t>
+  </si>
+  <si>
+    <t>CH_rw</t>
+  </si>
+  <si>
+    <t>IR_2</t>
+  </si>
+  <si>
+    <t>IRO_s2</t>
+  </si>
+  <si>
+    <t>IR1_s2</t>
+  </si>
+  <si>
+    <t>IR1_s1</t>
+  </si>
+  <si>
+    <t>IR0_s1</t>
+  </si>
+  <si>
+    <t>PC_ctrl[0]</t>
+  </si>
+  <si>
+    <t>PC_ctrl[1]</t>
+  </si>
+  <si>
+    <t>PCs_ctrl</t>
+  </si>
+  <si>
+    <t>DATA Memory</t>
+  </si>
+  <si>
+    <t>dmem_en</t>
+  </si>
+  <si>
+    <t>dmem_rw</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12</t>
+  </si>
+  <si>
+    <t>T13</t>
+  </si>
+  <si>
+    <t>T14</t>
+  </si>
+  <si>
+    <t>T15</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>T17</t>
+  </si>
+  <si>
+    <t>T18</t>
+  </si>
+  <si>
+    <t>T19</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>T21</t>
+  </si>
+  <si>
+    <t>T22</t>
+  </si>
+  <si>
+    <t>T23</t>
+  </si>
+  <si>
+    <t>T24</t>
+  </si>
+  <si>
+    <t>T25</t>
+  </si>
+  <si>
+    <t>T26</t>
+  </si>
+  <si>
+    <t>T27</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t>T29</t>
+  </si>
+  <si>
+    <t>T30</t>
+  </si>
+  <si>
+    <t>T31</t>
+  </si>
+  <si>
+    <t>T32</t>
+  </si>
+  <si>
+    <t>T33</t>
+  </si>
+  <si>
+    <t>T34</t>
+  </si>
+  <si>
+    <t>T35</t>
+  </si>
+  <si>
+    <t>T36</t>
+  </si>
+  <si>
+    <t>T37</t>
+  </si>
+  <si>
+    <t>T38</t>
+  </si>
+  <si>
+    <t>T39</t>
+  </si>
+  <si>
+    <t>T40</t>
+  </si>
+  <si>
+    <t>T41</t>
+  </si>
+  <si>
+    <t>T42</t>
+  </si>
+  <si>
+    <t>T43</t>
+  </si>
+  <si>
+    <t>T44</t>
+  </si>
+  <si>
+    <t>T45</t>
+  </si>
+  <si>
+    <t>T46</t>
+  </si>
+  <si>
+    <t>T47</t>
+  </si>
+  <si>
+    <t>T48</t>
+  </si>
+  <si>
+    <t>T49</t>
+  </si>
+  <si>
+    <t>T50</t>
   </si>
 </sst>
 </file>
@@ -151,18 +427,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -474,148 +753,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="11" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" customWidth="1"/>
+    <col min="11" max="11" width="5.7109375" customWidth="1"/>
     <col min="12" max="12" width="6.28515625" customWidth="1"/>
-    <col min="13" max="22" width="5.7109375" customWidth="1"/>
+    <col min="13" max="14" width="5.7109375" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" customWidth="1"/>
+    <col min="16" max="22" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="2:22" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="2:22" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-    </row>
-    <row r="3" spans="2:22" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="2:22" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -635,65 +922,486 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:U4"/>
+  <dimension ref="B2:AJ55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="B2:AJ55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" customWidth="1"/>
+    <col min="28" max="28" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:21" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="C2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+    </row>
+    <row r="3" spans="2:36" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="T3" s="6"/>
+      <c r="U3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-    </row>
-    <row r="3" spans="3:21" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="AC3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+    </row>
+    <row r="4" spans="2:36" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="3:21" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="3" t="s">
-        <v>30</v>
+      <c r="AC4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C2:U2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
+  <mergeCells count="10">
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AJ3"/>
+    <mergeCell ref="C2:S2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added control features to stage 55
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="137">
   <si>
     <t>PC</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>CP13</t>
+  </si>
+  <si>
+    <t>T55</t>
   </si>
 </sst>
 </file>
@@ -859,33 +862,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -897,6 +873,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1225,29 +1228,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
@@ -1257,43 +1260,43 @@
       <c r="B2" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="67" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67" t="s">
+      <c r="C2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67" t="s">
+      <c r="F2" s="71"/>
+      <c r="G2" s="71" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67" t="s">
+      <c r="H2" s="71"/>
+      <c r="I2" s="71" t="s">
         <v>115</v>
       </c>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="67"/>
+      <c r="L2" s="71"/>
       <c r="M2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="67" t="s">
+      <c r="N2" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67" t="s">
+      <c r="O2" s="71"/>
+      <c r="P2" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67" t="s">
+      <c r="Q2" s="71"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="71"/>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
@@ -2357,11 +2360,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK60"/>
+  <dimension ref="A1:AK61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R60" sqref="R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2391,44 +2394,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="79"/>
+      <c r="AC1" s="79"/>
+      <c r="AD1" s="79"/>
+      <c r="AE1" s="79"/>
+      <c r="AF1" s="79"/>
+      <c r="AG1" s="79"/>
+      <c r="AH1" s="79"/>
+      <c r="AI1" s="79"/>
+      <c r="AJ1" s="79"/>
     </row>
     <row r="2" spans="1:37" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="26" t="s">
@@ -2440,66 +2443,66 @@
       <c r="D2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="69" t="s">
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="71"/>
+      <c r="J2" s="74"/>
       <c r="K2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="69" t="s">
+      <c r="L2" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="71"/>
-      <c r="N2" s="70" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="71"/>
+      <c r="O2" s="74"/>
       <c r="P2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="69" t="s">
+      <c r="Q2" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="71"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="74"/>
       <c r="U2" s="20" t="s">
         <v>22</v>
       </c>
       <c r="V2" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="69" t="s">
+      <c r="W2" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="69" t="s">
+      <c r="X2" s="73"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="71"/>
+      <c r="AA2" s="74"/>
       <c r="AB2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="69" t="s">
+      <c r="AC2" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="71"/>
-      <c r="AF2" s="69" t="s">
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="AG2" s="70"/>
-      <c r="AH2" s="70"/>
-      <c r="AI2" s="70"/>
-      <c r="AJ2" s="71"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="73"/>
+      <c r="AJ2" s="74"/>
     </row>
     <row r="3" spans="1:37" s="2" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
@@ -8713,207 +8716,317 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:37" s="14" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="66" t="s">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="48">
+        <v>1</v>
+      </c>
+      <c r="C59" s="48">
+        <v>0</v>
+      </c>
+      <c r="D59" s="48">
+        <v>0</v>
+      </c>
+      <c r="E59" s="49">
+        <v>0</v>
+      </c>
+      <c r="F59" s="50">
+        <v>0</v>
+      </c>
+      <c r="G59" s="50">
+        <v>0</v>
+      </c>
+      <c r="H59" s="50">
+        <v>0</v>
+      </c>
+      <c r="I59" s="49">
+        <v>0</v>
+      </c>
+      <c r="J59" s="51">
+        <v>0</v>
+      </c>
+      <c r="K59" s="50">
+        <v>0</v>
+      </c>
+      <c r="L59" s="49">
+        <v>0</v>
+      </c>
+      <c r="M59" s="51">
+        <v>0</v>
+      </c>
+      <c r="N59" s="50">
+        <v>0</v>
+      </c>
+      <c r="O59" s="51">
+        <v>0</v>
+      </c>
+      <c r="P59" s="48">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="49">
+        <v>1</v>
+      </c>
+      <c r="R59" s="50">
+        <v>1</v>
+      </c>
+      <c r="S59" s="50">
+        <v>1</v>
+      </c>
+      <c r="T59" s="51">
+        <v>0</v>
+      </c>
+      <c r="U59" s="48">
+        <v>0</v>
+      </c>
+      <c r="V59" s="48">
+        <v>0</v>
+      </c>
+      <c r="W59" s="49">
+        <v>0</v>
+      </c>
+      <c r="X59" s="50">
+        <v>1</v>
+      </c>
+      <c r="Y59" s="51">
+        <v>1</v>
+      </c>
+      <c r="Z59" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA59" s="51">
+        <v>0</v>
+      </c>
+      <c r="AB59" s="48">
+        <v>1</v>
+      </c>
+      <c r="AC59" s="49">
+        <v>1</v>
+      </c>
+      <c r="AD59" s="50">
+        <v>0</v>
+      </c>
+      <c r="AE59" s="51">
+        <v>0</v>
+      </c>
+      <c r="AF59" s="49">
+        <v>0</v>
+      </c>
+      <c r="AG59" s="50">
+        <v>0</v>
+      </c>
+      <c r="AH59" s="50">
+        <v>0</v>
+      </c>
+      <c r="AI59" s="50">
+        <v>0</v>
+      </c>
+      <c r="AJ59" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37" s="14" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="C59" s="76" t="s">
+      <c r="C60" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="66" t="s">
+      <c r="D60" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="E59" s="77" t="s">
+      <c r="E60" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="F59" s="78" t="s">
+      <c r="F60" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="G59" s="78" t="s">
+      <c r="G60" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="H59" s="78" t="s">
+      <c r="H60" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="I59" s="77" t="s">
+      <c r="I60" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="J59" s="79" t="s">
+      <c r="J60" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="K59" s="78" t="s">
+      <c r="K60" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="L59" s="77" t="s">
+      <c r="L60" s="68" t="s">
         <v>134</v>
       </c>
-      <c r="M59" s="79" t="s">
+      <c r="M60" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="N59" s="78" t="s">
+      <c r="N60" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="O59" s="79" t="s">
+      <c r="O60" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="P59" s="66" t="s">
+      <c r="P60" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="Q59" s="77" t="s">
+      <c r="Q60" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="R59" s="78" t="s">
+      <c r="R60" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="S59" s="78" t="s">
+      <c r="S60" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="T59" s="79" t="s">
+      <c r="T60" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="U59" s="66" t="s">
+      <c r="U60" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="V59" s="66" t="s">
+      <c r="V60" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="W59" s="77" t="s">
+      <c r="W60" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="X59" s="78" t="s">
+      <c r="X60" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="Y59" s="79" t="s">
+      <c r="Y60" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="Z59" s="77" t="s">
+      <c r="Z60" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="AA59" s="79" t="s">
+      <c r="AA60" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="AB59" s="66" t="s">
+      <c r="AB60" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="AC59" s="77" t="s">
+      <c r="AC60" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="AD59" s="78" t="s">
+      <c r="AD60" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="AE59" s="79" t="s">
+      <c r="AE60" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="AF59" s="77" t="s">
+      <c r="AF60" s="68" t="s">
         <v>48</v>
       </c>
-      <c r="AG59" s="78" t="s">
+      <c r="AG60" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="AH59" s="78" t="s">
+      <c r="AH60" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="AI59" s="78" t="s">
+      <c r="AI60" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="AJ59" s="79" t="s">
+      <c r="AJ60" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AK59" s="15"/>
+      <c r="AK60" s="15"/>
     </row>
-    <row r="60" spans="1:37" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="27" t="s">
+    <row r="61" spans="1:37" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C61" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D61" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E60" s="73" t="s">
+      <c r="E61" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="F60" s="74"/>
-      <c r="G60" s="74"/>
-      <c r="H60" s="74"/>
-      <c r="I60" s="73" t="s">
+      <c r="F61" s="77"/>
+      <c r="G61" s="77"/>
+      <c r="H61" s="77"/>
+      <c r="I61" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="J60" s="75"/>
-      <c r="K60" s="29" t="s">
+      <c r="J61" s="78"/>
+      <c r="K61" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="L60" s="73" t="s">
+      <c r="L61" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M60" s="75"/>
-      <c r="N60" s="74" t="s">
+      <c r="M61" s="78"/>
+      <c r="N61" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="O60" s="75"/>
-      <c r="P60" s="22" t="s">
+      <c r="O61" s="78"/>
+      <c r="P61" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="Q60" s="73" t="s">
+      <c r="Q61" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="R60" s="74"/>
-      <c r="S60" s="74"/>
-      <c r="T60" s="75"/>
-      <c r="U60" s="22" t="s">
+      <c r="R61" s="77"/>
+      <c r="S61" s="77"/>
+      <c r="T61" s="78"/>
+      <c r="U61" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="V60" s="22" t="s">
+      <c r="V61" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="W60" s="73" t="s">
+      <c r="W61" s="76" t="s">
         <v>53</v>
       </c>
-      <c r="X60" s="74"/>
-      <c r="Y60" s="75"/>
-      <c r="Z60" s="73" t="s">
+      <c r="X61" s="77"/>
+      <c r="Y61" s="78"/>
+      <c r="Z61" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="AA60" s="75"/>
-      <c r="AB60" s="22" t="s">
+      <c r="AA61" s="78"/>
+      <c r="AB61" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AC60" s="73" t="s">
+      <c r="AC61" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="AD60" s="74"/>
-      <c r="AE60" s="75"/>
-      <c r="AF60" s="73" t="s">
+      <c r="AD61" s="77"/>
+      <c r="AE61" s="78"/>
+      <c r="AF61" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="AG60" s="74"/>
-      <c r="AH60" s="74"/>
-      <c r="AI60" s="74"/>
-      <c r="AJ60" s="75"/>
+      <c r="AG61" s="77"/>
+      <c r="AH61" s="77"/>
+      <c r="AI61" s="77"/>
+      <c r="AJ61" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="AF60:AJ60"/>
+    <mergeCell ref="AF61:AJ61"/>
     <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="A1:AJ1"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E60:H60"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="Q60:T60"/>
-    <mergeCell ref="W60:Y60"/>
-    <mergeCell ref="Z60:AA60"/>
-    <mergeCell ref="AC60:AE60"/>
+    <mergeCell ref="E61:H61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="Q61:T61"/>
+    <mergeCell ref="W61:Y61"/>
+    <mergeCell ref="Z61:AA61"/>
+    <mergeCell ref="AC61:AE61"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="L61:M61"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="54" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed dumb ALU bug - No MUX_ALU input for Instruction Register (OPERAND)
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -883,6 +883,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -891,15 +900,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2447,8 +2447,8 @@
   <dimension ref="A1:AK62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2527,66 +2527,66 @@
       <c r="D2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="77" t="s">
+      <c r="E2" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="77" t="s">
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="79"/>
+      <c r="J2" s="76"/>
       <c r="K2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="77" t="s">
+      <c r="L2" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="79"/>
-      <c r="N2" s="78" t="s">
+      <c r="M2" s="76"/>
+      <c r="N2" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="79"/>
+      <c r="O2" s="76"/>
       <c r="P2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="77" t="s">
+      <c r="Q2" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="79"/>
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="76"/>
       <c r="U2" s="18" t="s">
         <v>22</v>
       </c>
       <c r="V2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="77" t="s">
+      <c r="W2" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="77" t="s">
+      <c r="X2" s="75"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="79"/>
+      <c r="AA2" s="76"/>
       <c r="AB2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="77" t="s">
+      <c r="AC2" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="79"/>
-      <c r="AF2" s="77" t="s">
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="76"/>
+      <c r="AF2" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="79"/>
+      <c r="AG2" s="75"/>
+      <c r="AH2" s="75"/>
+      <c r="AI2" s="75"/>
+      <c r="AJ2" s="76"/>
     </row>
     <row r="3" spans="1:37" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="69">
@@ -4135,10 +4135,10 @@
         <v>1</v>
       </c>
       <c r="Z16" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA16" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB16" s="37">
         <v>1</v>
@@ -9170,74 +9170,69 @@
       <c r="D62" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E62" s="74" t="s">
+      <c r="E62" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="F62" s="75"/>
-      <c r="G62" s="75"/>
-      <c r="H62" s="75"/>
-      <c r="I62" s="74" t="s">
+      <c r="F62" s="78"/>
+      <c r="G62" s="78"/>
+      <c r="H62" s="78"/>
+      <c r="I62" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="J62" s="76"/>
+      <c r="J62" s="79"/>
       <c r="K62" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="L62" s="74" t="s">
+      <c r="L62" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="M62" s="76"/>
-      <c r="N62" s="75" t="s">
+      <c r="M62" s="79"/>
+      <c r="N62" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="O62" s="76"/>
+      <c r="O62" s="79"/>
       <c r="P62" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="Q62" s="74" t="s">
+      <c r="Q62" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="R62" s="75"/>
-      <c r="S62" s="75"/>
-      <c r="T62" s="76"/>
+      <c r="R62" s="78"/>
+      <c r="S62" s="78"/>
+      <c r="T62" s="79"/>
       <c r="U62" s="20" t="s">
         <v>22</v>
       </c>
       <c r="V62" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="W62" s="74" t="s">
+      <c r="W62" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="X62" s="75"/>
-      <c r="Y62" s="76"/>
-      <c r="Z62" s="74" t="s">
+      <c r="X62" s="78"/>
+      <c r="Y62" s="79"/>
+      <c r="Z62" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="AA62" s="76"/>
+      <c r="AA62" s="79"/>
       <c r="AB62" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AC62" s="74" t="s">
+      <c r="AC62" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="AD62" s="75"/>
-      <c r="AE62" s="76"/>
-      <c r="AF62" s="74" t="s">
+      <c r="AD62" s="78"/>
+      <c r="AE62" s="79"/>
+      <c r="AF62" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="AG62" s="75"/>
-      <c r="AH62" s="75"/>
-      <c r="AI62" s="75"/>
-      <c r="AJ62" s="76"/>
+      <c r="AG62" s="78"/>
+      <c r="AH62" s="78"/>
+      <c r="AI62" s="78"/>
+      <c r="AJ62" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="AF62:AJ62"/>
-    <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="A1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E62:H62"/>
@@ -9252,6 +9247,11 @@
     <mergeCell ref="L62:M62"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="AF62:AJ62"/>
+    <mergeCell ref="AF2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Added states for mult/div and shifting
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="146">
   <si>
     <t>PC</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>T63</t>
+  </si>
+  <si>
+    <t>T64</t>
   </si>
 </sst>
 </file>
@@ -904,10 +907,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2462,11 +2465,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK70"/>
+  <dimension ref="A1:AK71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:AJ68"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ69" sqref="A5:AJ69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2548,33 +2551,33 @@
       <c r="E2" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="74"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="26" t="s">
         <v>30</v>
       </c>
       <c r="L2" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="73" t="s">
+      <c r="M2" s="73"/>
+      <c r="N2" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="74"/>
+      <c r="O2" s="73"/>
       <c r="P2" s="18" t="s">
         <v>36</v>
       </c>
       <c r="Q2" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="73"/>
       <c r="U2" s="18" t="s">
         <v>22</v>
       </c>
@@ -2584,27 +2587,27 @@
       <c r="W2" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="73"/>
       <c r="Z2" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="74"/>
+      <c r="AA2" s="73"/>
       <c r="AB2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="AC2" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="74"/>
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="73"/>
       <c r="AF2" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="73"/>
-      <c r="AJ2" s="74"/>
+      <c r="AG2" s="74"/>
+      <c r="AH2" s="74"/>
+      <c r="AI2" s="74"/>
+      <c r="AJ2" s="73"/>
     </row>
     <row r="3" spans="1:37" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="65">
@@ -9070,112 +9073,112 @@
       </c>
     </row>
     <row r="61" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A61" s="40" t="s">
+      <c r="A61" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B61" s="37">
-        <v>1</v>
-      </c>
-      <c r="C61" s="37">
-        <v>0</v>
-      </c>
-      <c r="D61" s="37">
-        <v>0</v>
-      </c>
-      <c r="E61" s="38">
-        <v>0</v>
-      </c>
-      <c r="F61" s="36">
-        <v>0</v>
-      </c>
-      <c r="G61" s="36">
-        <v>0</v>
-      </c>
-      <c r="H61" s="36">
-        <v>0</v>
-      </c>
-      <c r="I61" s="38">
-        <v>0</v>
-      </c>
-      <c r="J61" s="39">
-        <v>0</v>
-      </c>
-      <c r="K61" s="36">
-        <v>0</v>
-      </c>
-      <c r="L61" s="38">
-        <v>0</v>
-      </c>
-      <c r="M61" s="39">
-        <v>0</v>
-      </c>
-      <c r="N61" s="36">
-        <v>0</v>
-      </c>
-      <c r="O61" s="39">
-        <v>0</v>
-      </c>
-      <c r="P61" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="38">
-        <v>1</v>
-      </c>
-      <c r="R61" s="36">
-        <v>0</v>
-      </c>
-      <c r="S61" s="36">
-        <v>1</v>
-      </c>
-      <c r="T61" s="39">
-        <v>0</v>
-      </c>
-      <c r="U61" s="37">
-        <v>0</v>
-      </c>
-      <c r="V61" s="37">
-        <v>0</v>
-      </c>
-      <c r="W61" s="38">
-        <v>0</v>
-      </c>
-      <c r="X61" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA61" s="39">
-        <v>0</v>
-      </c>
-      <c r="AB61" s="37">
-        <v>1</v>
-      </c>
-      <c r="AC61" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD61" s="36">
-        <v>0</v>
-      </c>
-      <c r="AE61" s="39">
-        <v>0</v>
-      </c>
-      <c r="AF61" s="38">
-        <v>1</v>
-      </c>
-      <c r="AG61" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH61" s="36">
-        <v>0</v>
-      </c>
-      <c r="AI61" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ61" s="39">
+      <c r="B61" s="42">
+        <v>1</v>
+      </c>
+      <c r="C61" s="42">
+        <v>0</v>
+      </c>
+      <c r="D61" s="42">
+        <v>0</v>
+      </c>
+      <c r="E61" s="43">
+        <v>0</v>
+      </c>
+      <c r="F61" s="44">
+        <v>0</v>
+      </c>
+      <c r="G61" s="44">
+        <v>0</v>
+      </c>
+      <c r="H61" s="44">
+        <v>0</v>
+      </c>
+      <c r="I61" s="43">
+        <v>0</v>
+      </c>
+      <c r="J61" s="45">
+        <v>0</v>
+      </c>
+      <c r="K61" s="44">
+        <v>0</v>
+      </c>
+      <c r="L61" s="43">
+        <v>0</v>
+      </c>
+      <c r="M61" s="45">
+        <v>0</v>
+      </c>
+      <c r="N61" s="44">
+        <v>0</v>
+      </c>
+      <c r="O61" s="45">
+        <v>0</v>
+      </c>
+      <c r="P61" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="43">
+        <v>1</v>
+      </c>
+      <c r="R61" s="44">
+        <v>1</v>
+      </c>
+      <c r="S61" s="44">
+        <v>1</v>
+      </c>
+      <c r="T61" s="45">
+        <v>0</v>
+      </c>
+      <c r="U61" s="42">
+        <v>0</v>
+      </c>
+      <c r="V61" s="42">
+        <v>0</v>
+      </c>
+      <c r="W61" s="43">
+        <v>0</v>
+      </c>
+      <c r="X61" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y61" s="45">
+        <v>1</v>
+      </c>
+      <c r="Z61" s="43">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="45">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC61" s="43">
+        <v>1</v>
+      </c>
+      <c r="AD61" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE61" s="45">
+        <v>0</v>
+      </c>
+      <c r="AF61" s="43">
+        <v>0</v>
+      </c>
+      <c r="AG61" s="44">
+        <v>0</v>
+      </c>
+      <c r="AH61" s="44">
+        <v>0</v>
+      </c>
+      <c r="AI61" s="44">
+        <v>0</v>
+      </c>
+      <c r="AJ61" s="45">
         <v>0</v>
       </c>
     </row>
@@ -9190,7 +9193,7 @@
         <v>0</v>
       </c>
       <c r="D62" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" s="38">
         <v>0</v>
@@ -9280,7 +9283,7 @@
         <v>0</v>
       </c>
       <c r="AH62" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI62" s="36">
         <v>0</v>
@@ -9288,7 +9291,6 @@
       <c r="AJ62" s="39">
         <v>0</v>
       </c>
-      <c r="AK62" s="69"/>
     </row>
     <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="40" t="s">
@@ -9388,10 +9390,10 @@
         <v>1</v>
       </c>
       <c r="AG63" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH63" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI63" s="36">
         <v>0</v>
@@ -9405,109 +9407,109 @@
       <c r="A64" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="B64" s="40">
-        <v>1</v>
-      </c>
-      <c r="C64" s="40">
-        <v>0</v>
-      </c>
-      <c r="D64" s="40">
-        <v>1</v>
-      </c>
-      <c r="E64" s="57">
-        <v>0</v>
-      </c>
-      <c r="F64" s="58">
-        <v>0</v>
-      </c>
-      <c r="G64" s="58">
-        <v>0</v>
-      </c>
-      <c r="H64" s="58">
-        <v>0</v>
-      </c>
-      <c r="I64" s="57">
-        <v>0</v>
-      </c>
-      <c r="J64" s="59">
-        <v>0</v>
-      </c>
-      <c r="K64" s="58">
-        <v>0</v>
-      </c>
-      <c r="L64" s="57">
-        <v>0</v>
-      </c>
-      <c r="M64" s="59">
-        <v>0</v>
-      </c>
-      <c r="N64" s="58">
-        <v>0</v>
-      </c>
-      <c r="O64" s="59">
-        <v>0</v>
-      </c>
-      <c r="P64" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="57">
-        <v>1</v>
-      </c>
-      <c r="R64" s="58">
-        <v>0</v>
-      </c>
-      <c r="S64" s="58">
-        <v>1</v>
-      </c>
-      <c r="T64" s="59">
-        <v>0</v>
-      </c>
-      <c r="U64" s="40">
-        <v>0</v>
-      </c>
-      <c r="V64" s="40">
-        <v>0</v>
-      </c>
-      <c r="W64" s="57">
-        <v>0</v>
-      </c>
-      <c r="X64" s="58">
-        <v>0</v>
-      </c>
-      <c r="Y64" s="59">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="57">
-        <v>1</v>
-      </c>
-      <c r="AA64" s="59">
-        <v>0</v>
-      </c>
-      <c r="AB64" s="40">
-        <v>1</v>
-      </c>
-      <c r="AC64" s="57">
-        <v>1</v>
-      </c>
-      <c r="AD64" s="58">
-        <v>0</v>
-      </c>
-      <c r="AE64" s="59">
-        <v>0</v>
-      </c>
-      <c r="AF64" s="57">
-        <v>1</v>
-      </c>
-      <c r="AG64" s="58">
-        <v>1</v>
-      </c>
-      <c r="AH64" s="58">
-        <v>0</v>
-      </c>
-      <c r="AI64" s="58">
-        <v>1</v>
-      </c>
-      <c r="AJ64" s="59">
+      <c r="B64" s="37">
+        <v>1</v>
+      </c>
+      <c r="C64" s="37">
+        <v>0</v>
+      </c>
+      <c r="D64" s="37">
+        <v>1</v>
+      </c>
+      <c r="E64" s="38">
+        <v>0</v>
+      </c>
+      <c r="F64" s="36">
+        <v>0</v>
+      </c>
+      <c r="G64" s="36">
+        <v>0</v>
+      </c>
+      <c r="H64" s="36">
+        <v>0</v>
+      </c>
+      <c r="I64" s="38">
+        <v>0</v>
+      </c>
+      <c r="J64" s="39">
+        <v>0</v>
+      </c>
+      <c r="K64" s="36">
+        <v>0</v>
+      </c>
+      <c r="L64" s="38">
+        <v>0</v>
+      </c>
+      <c r="M64" s="39">
+        <v>0</v>
+      </c>
+      <c r="N64" s="36">
+        <v>0</v>
+      </c>
+      <c r="O64" s="39">
+        <v>0</v>
+      </c>
+      <c r="P64" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="38">
+        <v>1</v>
+      </c>
+      <c r="R64" s="36">
+        <v>0</v>
+      </c>
+      <c r="S64" s="36">
+        <v>1</v>
+      </c>
+      <c r="T64" s="39">
+        <v>0</v>
+      </c>
+      <c r="U64" s="37">
+        <v>0</v>
+      </c>
+      <c r="V64" s="37">
+        <v>0</v>
+      </c>
+      <c r="W64" s="38">
+        <v>0</v>
+      </c>
+      <c r="X64" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA64" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC64" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD64" s="36">
+        <v>0</v>
+      </c>
+      <c r="AE64" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF64" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG64" s="36">
+        <v>1</v>
+      </c>
+      <c r="AH64" s="36">
+        <v>0</v>
+      </c>
+      <c r="AI64" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ64" s="39">
         <v>0</v>
       </c>
       <c r="AK64" s="69"/>
@@ -9516,109 +9518,109 @@
       <c r="A65" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="B65" s="37">
-        <v>1</v>
-      </c>
-      <c r="C65" s="37">
-        <v>0</v>
-      </c>
-      <c r="D65" s="37">
-        <v>0</v>
-      </c>
-      <c r="E65" s="38">
-        <v>0</v>
-      </c>
-      <c r="F65" s="36">
-        <v>0</v>
-      </c>
-      <c r="G65" s="36">
-        <v>0</v>
-      </c>
-      <c r="H65" s="36">
-        <v>0</v>
-      </c>
-      <c r="I65" s="38">
-        <v>0</v>
-      </c>
-      <c r="J65" s="39">
-        <v>0</v>
-      </c>
-      <c r="K65" s="36">
-        <v>0</v>
-      </c>
-      <c r="L65" s="38">
-        <v>0</v>
-      </c>
-      <c r="M65" s="39">
-        <v>0</v>
-      </c>
-      <c r="N65" s="36">
-        <v>0</v>
-      </c>
-      <c r="O65" s="39">
-        <v>0</v>
-      </c>
-      <c r="P65" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="38">
-        <v>1</v>
-      </c>
-      <c r="R65" s="36">
-        <v>0</v>
-      </c>
-      <c r="S65" s="36">
-        <v>1</v>
-      </c>
-      <c r="T65" s="39">
-        <v>0</v>
-      </c>
-      <c r="U65" s="37">
-        <v>0</v>
-      </c>
-      <c r="V65" s="37">
-        <v>0</v>
-      </c>
-      <c r="W65" s="38">
-        <v>0</v>
-      </c>
-      <c r="X65" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y65" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA65" s="39">
-        <v>0</v>
-      </c>
-      <c r="AB65" s="37">
-        <v>1</v>
-      </c>
-      <c r="AC65" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD65" s="36">
-        <v>0</v>
-      </c>
-      <c r="AE65" s="39">
-        <v>0</v>
-      </c>
-      <c r="AF65" s="38">
-        <v>1</v>
-      </c>
-      <c r="AG65" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH65" s="36">
-        <v>1</v>
-      </c>
-      <c r="AI65" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ65" s="39">
+      <c r="B65" s="40">
+        <v>1</v>
+      </c>
+      <c r="C65" s="40">
+        <v>0</v>
+      </c>
+      <c r="D65" s="40">
+        <v>1</v>
+      </c>
+      <c r="E65" s="57">
+        <v>0</v>
+      </c>
+      <c r="F65" s="58">
+        <v>0</v>
+      </c>
+      <c r="G65" s="58">
+        <v>0</v>
+      </c>
+      <c r="H65" s="58">
+        <v>0</v>
+      </c>
+      <c r="I65" s="57">
+        <v>0</v>
+      </c>
+      <c r="J65" s="59">
+        <v>0</v>
+      </c>
+      <c r="K65" s="58">
+        <v>0</v>
+      </c>
+      <c r="L65" s="57">
+        <v>0</v>
+      </c>
+      <c r="M65" s="59">
+        <v>0</v>
+      </c>
+      <c r="N65" s="58">
+        <v>0</v>
+      </c>
+      <c r="O65" s="59">
+        <v>0</v>
+      </c>
+      <c r="P65" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="57">
+        <v>1</v>
+      </c>
+      <c r="R65" s="58">
+        <v>0</v>
+      </c>
+      <c r="S65" s="58">
+        <v>1</v>
+      </c>
+      <c r="T65" s="59">
+        <v>0</v>
+      </c>
+      <c r="U65" s="40">
+        <v>0</v>
+      </c>
+      <c r="V65" s="40">
+        <v>0</v>
+      </c>
+      <c r="W65" s="57">
+        <v>0</v>
+      </c>
+      <c r="X65" s="58">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="57">
+        <v>1</v>
+      </c>
+      <c r="AA65" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="40">
+        <v>1</v>
+      </c>
+      <c r="AC65" s="57">
+        <v>1</v>
+      </c>
+      <c r="AD65" s="58">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="57">
+        <v>1</v>
+      </c>
+      <c r="AG65" s="58">
+        <v>1</v>
+      </c>
+      <c r="AH65" s="58">
+        <v>0</v>
+      </c>
+      <c r="AI65" s="58">
+        <v>1</v>
+      </c>
+      <c r="AJ65" s="59">
         <v>0</v>
       </c>
       <c r="AK65" s="69"/>
@@ -9832,13 +9834,13 @@
         <v>1</v>
       </c>
       <c r="AG67" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH67" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI67" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ67" s="39">
         <v>0</v>
@@ -9954,209 +9956,320 @@
       <c r="AJ68" s="39">
         <v>0</v>
       </c>
-      <c r="AK68" s="68"/>
+      <c r="AK68" s="69"/>
     </row>
-    <row r="69" spans="1:37" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17"/>
-      <c r="B69" s="60" t="s">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A69" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" s="37">
+        <v>1</v>
+      </c>
+      <c r="C69" s="37">
+        <v>0</v>
+      </c>
+      <c r="D69" s="37">
+        <v>0</v>
+      </c>
+      <c r="E69" s="38">
+        <v>0</v>
+      </c>
+      <c r="F69" s="36">
+        <v>0</v>
+      </c>
+      <c r="G69" s="36">
+        <v>0</v>
+      </c>
+      <c r="H69" s="36">
+        <v>0</v>
+      </c>
+      <c r="I69" s="38">
+        <v>0</v>
+      </c>
+      <c r="J69" s="39">
+        <v>0</v>
+      </c>
+      <c r="K69" s="36">
+        <v>0</v>
+      </c>
+      <c r="L69" s="38">
+        <v>0</v>
+      </c>
+      <c r="M69" s="39">
+        <v>0</v>
+      </c>
+      <c r="N69" s="36">
+        <v>0</v>
+      </c>
+      <c r="O69" s="39">
+        <v>0</v>
+      </c>
+      <c r="P69" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="38">
+        <v>1</v>
+      </c>
+      <c r="R69" s="36">
+        <v>0</v>
+      </c>
+      <c r="S69" s="36">
+        <v>1</v>
+      </c>
+      <c r="T69" s="39">
+        <v>0</v>
+      </c>
+      <c r="U69" s="37">
+        <v>0</v>
+      </c>
+      <c r="V69" s="37">
+        <v>0</v>
+      </c>
+      <c r="W69" s="38">
+        <v>0</v>
+      </c>
+      <c r="X69" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z69" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA69" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB69" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC69" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD69" s="36">
+        <v>0</v>
+      </c>
+      <c r="AE69" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF69" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG69" s="36">
+        <v>1</v>
+      </c>
+      <c r="AH69" s="36">
+        <v>0</v>
+      </c>
+      <c r="AI69" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ69" s="39">
+        <v>0</v>
+      </c>
+      <c r="AK69" s="68"/>
+    </row>
+    <row r="70" spans="1:37" s="12" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="17"/>
+      <c r="B70" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="C69" s="61" t="s">
+      <c r="C70" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="D69" s="60" t="s">
+      <c r="D70" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="E69" s="62" t="s">
+      <c r="E70" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="F69" s="63" t="s">
+      <c r="F70" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="G69" s="63" t="s">
+      <c r="G70" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="H69" s="63" t="s">
+      <c r="H70" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="I69" s="62" t="s">
+      <c r="I70" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="J69" s="64" t="s">
+      <c r="J70" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="K69" s="63" t="s">
+      <c r="K70" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="L69" s="62" t="s">
+      <c r="L70" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="M69" s="64" t="s">
+      <c r="M70" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="N69" s="63" t="s">
+      <c r="N70" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="O69" s="64" t="s">
+      <c r="O70" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="P69" s="60" t="s">
+      <c r="P70" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="Q69" s="62" t="s">
+      <c r="Q70" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="R69" s="63" t="s">
+      <c r="R70" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="S69" s="63" t="s">
+      <c r="S70" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="T69" s="64" t="s">
+      <c r="T70" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="U69" s="60" t="s">
+      <c r="U70" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="V69" s="60" t="s">
+      <c r="V70" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="W69" s="62" t="s">
+      <c r="W70" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="X69" s="63" t="s">
+      <c r="X70" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="Y69" s="64" t="s">
+      <c r="Y70" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="Z69" s="62" t="s">
+      <c r="Z70" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="AA69" s="64" t="s">
+      <c r="AA70" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="AB69" s="60" t="s">
+      <c r="AB70" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="AC69" s="62" t="s">
+      <c r="AC70" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AD69" s="63" t="s">
+      <c r="AD70" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="AE69" s="64" t="s">
+      <c r="AE70" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="AF69" s="62" t="s">
+      <c r="AF70" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="AG69" s="63" t="s">
+      <c r="AG70" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="AH69" s="63" t="s">
+      <c r="AH70" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="AI69" s="63" t="s">
+      <c r="AI70" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="AJ69" s="64" t="s">
+      <c r="AJ70" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AK69" s="13"/>
+      <c r="AK70" s="13"/>
     </row>
-    <row r="70" spans="1:37" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="25" t="s">
+    <row r="71" spans="1:37" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="C70" s="23" t="s">
+      <c r="C71" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D70" s="20" t="s">
+      <c r="D71" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E70" s="75" t="s">
+      <c r="E71" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="F70" s="76"/>
-      <c r="G70" s="76"/>
-      <c r="H70" s="76"/>
-      <c r="I70" s="75" t="s">
+      <c r="F71" s="76"/>
+      <c r="G71" s="76"/>
+      <c r="H71" s="76"/>
+      <c r="I71" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="J70" s="77"/>
-      <c r="K70" s="27" t="s">
+      <c r="J71" s="77"/>
+      <c r="K71" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="L70" s="75" t="s">
+      <c r="L71" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="M70" s="77"/>
-      <c r="N70" s="76" t="s">
+      <c r="M71" s="77"/>
+      <c r="N71" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="O70" s="77"/>
-      <c r="P70" s="20" t="s">
+      <c r="O71" s="77"/>
+      <c r="P71" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="Q70" s="75" t="s">
+      <c r="Q71" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="R70" s="76"/>
-      <c r="S70" s="76"/>
-      <c r="T70" s="77"/>
-      <c r="U70" s="20" t="s">
+      <c r="R71" s="76"/>
+      <c r="S71" s="76"/>
+      <c r="T71" s="77"/>
+      <c r="U71" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="V70" s="20" t="s">
+      <c r="V71" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="W70" s="75" t="s">
+      <c r="W71" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="X70" s="76"/>
-      <c r="Y70" s="77"/>
-      <c r="Z70" s="75" t="s">
+      <c r="X71" s="76"/>
+      <c r="Y71" s="77"/>
+      <c r="Z71" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="AA70" s="77"/>
-      <c r="AB70" s="20" t="s">
+      <c r="AA71" s="77"/>
+      <c r="AB71" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AC70" s="75" t="s">
+      <c r="AC71" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="AD70" s="76"/>
-      <c r="AE70" s="77"/>
-      <c r="AF70" s="75" t="s">
+      <c r="AD71" s="76"/>
+      <c r="AE71" s="77"/>
+      <c r="AF71" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="AG70" s="76"/>
-      <c r="AH70" s="76"/>
-      <c r="AI70" s="76"/>
-      <c r="AJ70" s="77"/>
+      <c r="AG71" s="76"/>
+      <c r="AH71" s="76"/>
+      <c r="AI71" s="76"/>
+      <c r="AJ71" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:AJ1"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="N71:O71"/>
+    <mergeCell ref="Q71:T71"/>
+    <mergeCell ref="W71:Y71"/>
+    <mergeCell ref="Z71:AA71"/>
+    <mergeCell ref="AC71:AE71"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="L71:M71"/>
+    <mergeCell ref="W2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="AF70:AJ70"/>
+    <mergeCell ref="AF71:AJ71"/>
     <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="A1:AJ1"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E70:H70"/>
-    <mergeCell ref="N70:O70"/>
-    <mergeCell ref="Q70:T70"/>
-    <mergeCell ref="W70:Y70"/>
-    <mergeCell ref="Z70:AA70"/>
-    <mergeCell ref="AC70:AE70"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="L70:M70"/>
-    <mergeCell ref="W2:Y2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11110,10 +11223,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ64"/>
+  <dimension ref="A1:AJ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AJ65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17283,117 +17396,117 @@
       </c>
     </row>
     <row r="57" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B57" s="37">
-        <v>1</v>
-      </c>
-      <c r="C57" s="37">
-        <v>0</v>
-      </c>
-      <c r="D57" s="37">
-        <v>0</v>
-      </c>
-      <c r="E57" s="38">
-        <v>0</v>
-      </c>
-      <c r="F57" s="36">
-        <v>0</v>
-      </c>
-      <c r="G57" s="36">
-        <v>0</v>
-      </c>
-      <c r="H57" s="36">
-        <v>0</v>
-      </c>
-      <c r="I57" s="38">
-        <v>0</v>
-      </c>
-      <c r="J57" s="39">
-        <v>0</v>
-      </c>
-      <c r="K57" s="36">
-        <v>0</v>
-      </c>
-      <c r="L57" s="38">
-        <v>0</v>
-      </c>
-      <c r="M57" s="39">
-        <v>0</v>
-      </c>
-      <c r="N57" s="36">
-        <v>0</v>
-      </c>
-      <c r="O57" s="39">
-        <v>0</v>
-      </c>
-      <c r="P57" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="38">
-        <v>1</v>
-      </c>
-      <c r="R57" s="36">
-        <v>0</v>
-      </c>
-      <c r="S57" s="36">
-        <v>1</v>
-      </c>
-      <c r="T57" s="39">
-        <v>0</v>
-      </c>
-      <c r="U57" s="37">
-        <v>0</v>
-      </c>
-      <c r="V57" s="37">
-        <v>0</v>
-      </c>
-      <c r="W57" s="38">
-        <v>0</v>
-      </c>
-      <c r="X57" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA57" s="39">
-        <v>0</v>
-      </c>
-      <c r="AB57" s="37">
-        <v>1</v>
-      </c>
-      <c r="AC57" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD57" s="36">
-        <v>0</v>
-      </c>
-      <c r="AE57" s="39">
-        <v>0</v>
-      </c>
-      <c r="AF57" s="38">
-        <v>1</v>
-      </c>
-      <c r="AG57" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH57" s="36">
-        <v>0</v>
-      </c>
-      <c r="AI57" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ57" s="39">
+      <c r="B57" s="42">
+        <v>1</v>
+      </c>
+      <c r="C57" s="42">
+        <v>0</v>
+      </c>
+      <c r="D57" s="42">
+        <v>0</v>
+      </c>
+      <c r="E57" s="43">
+        <v>0</v>
+      </c>
+      <c r="F57" s="44">
+        <v>0</v>
+      </c>
+      <c r="G57" s="44">
+        <v>0</v>
+      </c>
+      <c r="H57" s="44">
+        <v>0</v>
+      </c>
+      <c r="I57" s="43">
+        <v>0</v>
+      </c>
+      <c r="J57" s="45">
+        <v>0</v>
+      </c>
+      <c r="K57" s="44">
+        <v>0</v>
+      </c>
+      <c r="L57" s="43">
+        <v>0</v>
+      </c>
+      <c r="M57" s="45">
+        <v>0</v>
+      </c>
+      <c r="N57" s="44">
+        <v>0</v>
+      </c>
+      <c r="O57" s="45">
+        <v>0</v>
+      </c>
+      <c r="P57" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="43">
+        <v>1</v>
+      </c>
+      <c r="R57" s="44">
+        <v>1</v>
+      </c>
+      <c r="S57" s="44">
+        <v>1</v>
+      </c>
+      <c r="T57" s="45">
+        <v>0</v>
+      </c>
+      <c r="U57" s="42">
+        <v>0</v>
+      </c>
+      <c r="V57" s="42">
+        <v>0</v>
+      </c>
+      <c r="W57" s="43">
+        <v>0</v>
+      </c>
+      <c r="X57" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="45">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="43">
+        <v>1</v>
+      </c>
+      <c r="AA57" s="45">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="42">
+        <v>1</v>
+      </c>
+      <c r="AC57" s="43">
+        <v>1</v>
+      </c>
+      <c r="AD57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE57" s="45">
+        <v>0</v>
+      </c>
+      <c r="AF57" s="43">
+        <v>0</v>
+      </c>
+      <c r="AG57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AH57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AI57" s="44">
+        <v>0</v>
+      </c>
+      <c r="AJ57" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="40" t="s">
         <v>138</v>
       </c>
       <c r="B58" s="37">
@@ -17403,7 +17516,7 @@
         <v>0</v>
       </c>
       <c r="D58" s="37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" s="38">
         <v>0</v>
@@ -17493,7 +17606,7 @@
         <v>0</v>
       </c>
       <c r="AH58" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI58" s="36">
         <v>0</v>
@@ -17503,7 +17616,7 @@
       </c>
     </row>
     <row r="59" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="40" t="s">
         <v>139</v>
       </c>
       <c r="B59" s="37">
@@ -17600,10 +17713,10 @@
         <v>1</v>
       </c>
       <c r="AG59" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH59" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI59" s="36">
         <v>0</v>
@@ -17613,227 +17726,227 @@
       </c>
     </row>
     <row r="60" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="40">
-        <v>1</v>
-      </c>
-      <c r="C60" s="40">
-        <v>0</v>
-      </c>
-      <c r="D60" s="40">
-        <v>1</v>
-      </c>
-      <c r="E60" s="57">
-        <v>0</v>
-      </c>
-      <c r="F60" s="58">
-        <v>0</v>
-      </c>
-      <c r="G60" s="58">
-        <v>0</v>
-      </c>
-      <c r="H60" s="58">
-        <v>0</v>
-      </c>
-      <c r="I60" s="57">
-        <v>0</v>
-      </c>
-      <c r="J60" s="59">
-        <v>0</v>
-      </c>
-      <c r="K60" s="58">
-        <v>0</v>
-      </c>
-      <c r="L60" s="57">
-        <v>0</v>
-      </c>
-      <c r="M60" s="59">
-        <v>0</v>
-      </c>
-      <c r="N60" s="58">
-        <v>0</v>
-      </c>
-      <c r="O60" s="59">
-        <v>0</v>
-      </c>
-      <c r="P60" s="40">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="57">
-        <v>1</v>
-      </c>
-      <c r="R60" s="58">
-        <v>0</v>
-      </c>
-      <c r="S60" s="58">
-        <v>1</v>
-      </c>
-      <c r="T60" s="59">
-        <v>0</v>
-      </c>
-      <c r="U60" s="40">
-        <v>0</v>
-      </c>
-      <c r="V60" s="40">
-        <v>0</v>
-      </c>
-      <c r="W60" s="57">
-        <v>0</v>
-      </c>
-      <c r="X60" s="58">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="59">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="57">
-        <v>1</v>
-      </c>
-      <c r="AA60" s="59">
-        <v>0</v>
-      </c>
-      <c r="AB60" s="40">
-        <v>1</v>
-      </c>
-      <c r="AC60" s="57">
-        <v>1</v>
-      </c>
-      <c r="AD60" s="58">
-        <v>0</v>
-      </c>
-      <c r="AE60" s="59">
-        <v>0</v>
-      </c>
-      <c r="AF60" s="57">
-        <v>1</v>
-      </c>
-      <c r="AG60" s="58">
-        <v>1</v>
-      </c>
-      <c r="AH60" s="58">
-        <v>0</v>
-      </c>
-      <c r="AI60" s="58">
-        <v>1</v>
-      </c>
-      <c r="AJ60" s="59">
+      <c r="B60" s="37">
+        <v>1</v>
+      </c>
+      <c r="C60" s="37">
+        <v>0</v>
+      </c>
+      <c r="D60" s="37">
+        <v>1</v>
+      </c>
+      <c r="E60" s="38">
+        <v>0</v>
+      </c>
+      <c r="F60" s="36">
+        <v>0</v>
+      </c>
+      <c r="G60" s="36">
+        <v>0</v>
+      </c>
+      <c r="H60" s="36">
+        <v>0</v>
+      </c>
+      <c r="I60" s="38">
+        <v>0</v>
+      </c>
+      <c r="J60" s="39">
+        <v>0</v>
+      </c>
+      <c r="K60" s="36">
+        <v>0</v>
+      </c>
+      <c r="L60" s="38">
+        <v>0</v>
+      </c>
+      <c r="M60" s="39">
+        <v>0</v>
+      </c>
+      <c r="N60" s="36">
+        <v>0</v>
+      </c>
+      <c r="O60" s="39">
+        <v>0</v>
+      </c>
+      <c r="P60" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="38">
+        <v>1</v>
+      </c>
+      <c r="R60" s="36">
+        <v>0</v>
+      </c>
+      <c r="S60" s="36">
+        <v>1</v>
+      </c>
+      <c r="T60" s="39">
+        <v>0</v>
+      </c>
+      <c r="U60" s="37">
+        <v>0</v>
+      </c>
+      <c r="V60" s="37">
+        <v>0</v>
+      </c>
+      <c r="W60" s="38">
+        <v>0</v>
+      </c>
+      <c r="X60" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA60" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC60" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD60" s="36">
+        <v>0</v>
+      </c>
+      <c r="AE60" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF60" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG60" s="36">
+        <v>1</v>
+      </c>
+      <c r="AH60" s="36">
+        <v>0</v>
+      </c>
+      <c r="AI60" s="36">
+        <v>0</v>
+      </c>
+      <c r="AJ60" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A61" s="28" t="s">
+      <c r="A61" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="B61" s="37">
-        <v>1</v>
-      </c>
-      <c r="C61" s="37">
-        <v>0</v>
-      </c>
-      <c r="D61" s="37">
-        <v>0</v>
-      </c>
-      <c r="E61" s="38">
-        <v>0</v>
-      </c>
-      <c r="F61" s="36">
-        <v>0</v>
-      </c>
-      <c r="G61" s="36">
-        <v>0</v>
-      </c>
-      <c r="H61" s="36">
-        <v>0</v>
-      </c>
-      <c r="I61" s="38">
-        <v>0</v>
-      </c>
-      <c r="J61" s="39">
-        <v>0</v>
-      </c>
-      <c r="K61" s="36">
-        <v>0</v>
-      </c>
-      <c r="L61" s="38">
-        <v>0</v>
-      </c>
-      <c r="M61" s="39">
-        <v>0</v>
-      </c>
-      <c r="N61" s="36">
-        <v>0</v>
-      </c>
-      <c r="O61" s="39">
-        <v>0</v>
-      </c>
-      <c r="P61" s="37">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="38">
-        <v>1</v>
-      </c>
-      <c r="R61" s="36">
-        <v>0</v>
-      </c>
-      <c r="S61" s="36">
-        <v>1</v>
-      </c>
-      <c r="T61" s="39">
-        <v>0</v>
-      </c>
-      <c r="U61" s="37">
-        <v>0</v>
-      </c>
-      <c r="V61" s="37">
-        <v>0</v>
-      </c>
-      <c r="W61" s="38">
-        <v>0</v>
-      </c>
-      <c r="X61" s="36">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="39">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="38">
-        <v>1</v>
-      </c>
-      <c r="AA61" s="39">
-        <v>0</v>
-      </c>
-      <c r="AB61" s="37">
-        <v>1</v>
-      </c>
-      <c r="AC61" s="38">
-        <v>1</v>
-      </c>
-      <c r="AD61" s="36">
-        <v>0</v>
-      </c>
-      <c r="AE61" s="39">
-        <v>0</v>
-      </c>
-      <c r="AF61" s="38">
-        <v>1</v>
-      </c>
-      <c r="AG61" s="36">
-        <v>0</v>
-      </c>
-      <c r="AH61" s="36">
-        <v>1</v>
-      </c>
-      <c r="AI61" s="36">
-        <v>0</v>
-      </c>
-      <c r="AJ61" s="39">
+      <c r="B61" s="40">
+        <v>1</v>
+      </c>
+      <c r="C61" s="40">
+        <v>0</v>
+      </c>
+      <c r="D61" s="40">
+        <v>1</v>
+      </c>
+      <c r="E61" s="57">
+        <v>0</v>
+      </c>
+      <c r="F61" s="58">
+        <v>0</v>
+      </c>
+      <c r="G61" s="58">
+        <v>0</v>
+      </c>
+      <c r="H61" s="58">
+        <v>0</v>
+      </c>
+      <c r="I61" s="57">
+        <v>0</v>
+      </c>
+      <c r="J61" s="59">
+        <v>0</v>
+      </c>
+      <c r="K61" s="58">
+        <v>0</v>
+      </c>
+      <c r="L61" s="57">
+        <v>0</v>
+      </c>
+      <c r="M61" s="59">
+        <v>0</v>
+      </c>
+      <c r="N61" s="58">
+        <v>0</v>
+      </c>
+      <c r="O61" s="59">
+        <v>0</v>
+      </c>
+      <c r="P61" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="57">
+        <v>1</v>
+      </c>
+      <c r="R61" s="58">
+        <v>0</v>
+      </c>
+      <c r="S61" s="58">
+        <v>1</v>
+      </c>
+      <c r="T61" s="59">
+        <v>0</v>
+      </c>
+      <c r="U61" s="40">
+        <v>0</v>
+      </c>
+      <c r="V61" s="40">
+        <v>0</v>
+      </c>
+      <c r="W61" s="57">
+        <v>0</v>
+      </c>
+      <c r="X61" s="58">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="59">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="57">
+        <v>1</v>
+      </c>
+      <c r="AA61" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="40">
+        <v>1</v>
+      </c>
+      <c r="AC61" s="57">
+        <v>1</v>
+      </c>
+      <c r="AD61" s="58">
+        <v>0</v>
+      </c>
+      <c r="AE61" s="59">
+        <v>0</v>
+      </c>
+      <c r="AF61" s="57">
+        <v>1</v>
+      </c>
+      <c r="AG61" s="58">
+        <v>1</v>
+      </c>
+      <c r="AH61" s="58">
+        <v>0</v>
+      </c>
+      <c r="AI61" s="58">
+        <v>1</v>
+      </c>
+      <c r="AJ61" s="59">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A62" s="28" t="s">
+      <c r="A62" s="40" t="s">
         <v>142</v>
       </c>
       <c r="B62" s="37">
@@ -17943,7 +18056,7 @@
       </c>
     </row>
     <row r="63" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="40" t="s">
         <v>143</v>
       </c>
       <c r="B63" s="37">
@@ -18040,20 +18153,20 @@
         <v>1</v>
       </c>
       <c r="AG63" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH63" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI63" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ63" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A64" s="28" t="s">
+      <c r="A64" s="40" t="s">
         <v>144</v>
       </c>
       <c r="B64" s="37">
@@ -18159,6 +18272,116 @@
         <v>1</v>
       </c>
       <c r="AJ64" s="39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A65" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" s="37">
+        <v>1</v>
+      </c>
+      <c r="C65" s="37">
+        <v>0</v>
+      </c>
+      <c r="D65" s="37">
+        <v>0</v>
+      </c>
+      <c r="E65" s="38">
+        <v>0</v>
+      </c>
+      <c r="F65" s="36">
+        <v>0</v>
+      </c>
+      <c r="G65" s="36">
+        <v>0</v>
+      </c>
+      <c r="H65" s="36">
+        <v>0</v>
+      </c>
+      <c r="I65" s="38">
+        <v>0</v>
+      </c>
+      <c r="J65" s="39">
+        <v>0</v>
+      </c>
+      <c r="K65" s="36">
+        <v>0</v>
+      </c>
+      <c r="L65" s="38">
+        <v>0</v>
+      </c>
+      <c r="M65" s="39">
+        <v>0</v>
+      </c>
+      <c r="N65" s="36">
+        <v>0</v>
+      </c>
+      <c r="O65" s="39">
+        <v>0</v>
+      </c>
+      <c r="P65" s="37">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="38">
+        <v>1</v>
+      </c>
+      <c r="R65" s="36">
+        <v>0</v>
+      </c>
+      <c r="S65" s="36">
+        <v>1</v>
+      </c>
+      <c r="T65" s="39">
+        <v>0</v>
+      </c>
+      <c r="U65" s="37">
+        <v>0</v>
+      </c>
+      <c r="V65" s="37">
+        <v>0</v>
+      </c>
+      <c r="W65" s="38">
+        <v>0</v>
+      </c>
+      <c r="X65" s="36">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="39">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="38">
+        <v>1</v>
+      </c>
+      <c r="AA65" s="39">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC65" s="38">
+        <v>1</v>
+      </c>
+      <c r="AD65" s="36">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="39">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG65" s="36">
+        <v>1</v>
+      </c>
+      <c r="AH65" s="36">
+        <v>0</v>
+      </c>
+      <c r="AI65" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ65" s="39">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ALU + MULTDIV Working
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -904,13 +904,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -922,8 +922,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2468,8 +2468,8 @@
   <dimension ref="A1:AK71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ69" sqref="A5:AJ69"/>
+      <pane ySplit="4" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:AJ69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2499,44 +2499,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
+      <c r="AG1" s="78"/>
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
     </row>
     <row r="2" spans="1:37" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
@@ -2548,66 +2548,66 @@
       <c r="D2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="73" t="s">
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="78"/>
+      <c r="J2" s="74"/>
       <c r="K2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="73" t="s">
+      <c r="L2" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="78"/>
-      <c r="N2" s="74" t="s">
+      <c r="M2" s="74"/>
+      <c r="N2" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="78"/>
+      <c r="O2" s="74"/>
       <c r="P2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="73" t="s">
+      <c r="Q2" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="78"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="74"/>
       <c r="U2" s="18" t="s">
         <v>22</v>
       </c>
       <c r="V2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="73" t="s">
+      <c r="W2" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="73" t="s">
+      <c r="X2" s="73"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="78"/>
+      <c r="AA2" s="74"/>
       <c r="AB2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="73" t="s">
+      <c r="AC2" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="74"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="73" t="s">
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="AG2" s="74"/>
-      <c r="AH2" s="74"/>
-      <c r="AI2" s="74"/>
-      <c r="AJ2" s="78"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="73"/>
+      <c r="AJ2" s="74"/>
     </row>
     <row r="3" spans="1:37" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="65">
@@ -5173,13 +5173,13 @@
         <v>0</v>
       </c>
       <c r="AF25" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG25" s="36">
         <v>0</v>
       </c>
       <c r="AH25" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI25" s="36">
         <v>0</v>
@@ -5395,13 +5395,13 @@
         <v>0</v>
       </c>
       <c r="AF27" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG27" s="36">
         <v>0</v>
       </c>
       <c r="AH27" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI27" s="36">
         <v>0</v>
@@ -5617,16 +5617,16 @@
         <v>0</v>
       </c>
       <c r="AF29" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG29" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH29" s="36">
         <v>0</v>
       </c>
       <c r="AI29" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ29" s="35">
         <v>1</v>
@@ -5839,16 +5839,16 @@
         <v>0</v>
       </c>
       <c r="AF31" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG31" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH31" s="36">
         <v>0</v>
       </c>
       <c r="AI31" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ31" s="35">
         <v>1</v>
@@ -6061,7 +6061,7 @@
         <v>0</v>
       </c>
       <c r="AF33" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG33" s="36">
         <v>0</v>
@@ -6172,13 +6172,13 @@
         <v>0</v>
       </c>
       <c r="AF34" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG34" s="36">
         <v>0</v>
       </c>
       <c r="AH34" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI34" s="36">
         <v>0</v>
@@ -6283,10 +6283,10 @@
         <v>0</v>
       </c>
       <c r="AF35" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG35" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH35" s="36">
         <v>0</v>
@@ -6394,16 +6394,16 @@
         <v>0</v>
       </c>
       <c r="AF36" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG36" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH36" s="32">
         <v>0</v>
       </c>
       <c r="AI36" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ36" s="35">
         <v>1</v>
@@ -9726,7 +9726,7 @@
         <v>0</v>
       </c>
       <c r="AH66" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI66" s="36">
         <v>0</v>
@@ -9837,7 +9837,7 @@
         <v>0</v>
       </c>
       <c r="AH67" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI67" s="36">
         <v>0</v>
@@ -9951,7 +9951,7 @@
         <v>0</v>
       </c>
       <c r="AI68" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ68" s="35">
         <v>1</v>
@@ -10062,7 +10062,7 @@
         <v>0</v>
       </c>
       <c r="AI69" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ69" s="35">
         <v>1</v>
@@ -10251,6 +10251,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="AF71:AJ71"/>
     <mergeCell ref="AF2:AJ2"/>
@@ -10267,9 +10270,6 @@
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="L71:M71"/>
     <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11225,7 +11225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:AJ65"/>
     </sheetView>
   </sheetViews>
@@ -13530,13 +13530,13 @@
         <v>0</v>
       </c>
       <c r="AF21" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG21" s="36">
         <v>0</v>
       </c>
       <c r="AH21" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI21" s="36">
         <v>0</v>
@@ -13750,13 +13750,13 @@
         <v>0</v>
       </c>
       <c r="AF23" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG23" s="36">
         <v>0</v>
       </c>
       <c r="AH23" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI23" s="36">
         <v>0</v>
@@ -13970,16 +13970,16 @@
         <v>0</v>
       </c>
       <c r="AF25" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG25" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH25" s="36">
         <v>0</v>
       </c>
       <c r="AI25" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ25" s="35">
         <v>1</v>
@@ -14190,16 +14190,16 @@
         <v>0</v>
       </c>
       <c r="AF27" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG27" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH27" s="36">
         <v>0</v>
       </c>
       <c r="AI27" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27" s="35">
         <v>1</v>
@@ -14410,7 +14410,7 @@
         <v>0</v>
       </c>
       <c r="AF29" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG29" s="36">
         <v>0</v>
@@ -14520,13 +14520,13 @@
         <v>0</v>
       </c>
       <c r="AF30" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG30" s="36">
         <v>0</v>
       </c>
       <c r="AH30" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI30" s="36">
         <v>0</v>
@@ -14630,10 +14630,10 @@
         <v>0</v>
       </c>
       <c r="AF31" s="38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG31" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH31" s="36">
         <v>0</v>
@@ -14740,16 +14740,16 @@
         <v>0</v>
       </c>
       <c r="AF32" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG32" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH32" s="32">
         <v>0</v>
       </c>
       <c r="AI32" s="32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ32" s="35">
         <v>1</v>
@@ -18046,7 +18046,7 @@
         <v>0</v>
       </c>
       <c r="AH62" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI62" s="36">
         <v>0</v>
@@ -18156,7 +18156,7 @@
         <v>0</v>
       </c>
       <c r="AH63" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI63" s="36">
         <v>0</v>
@@ -18269,7 +18269,7 @@
         <v>0</v>
       </c>
       <c r="AI64" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ64" s="35">
         <v>1</v>
@@ -18379,7 +18379,7 @@
         <v>0</v>
       </c>
       <c r="AI65" s="36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ65" s="35">
         <v>1</v>

</xml_diff>

<commit_message>
Working out kinks in divide. About to do something bold with cache
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="10545" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19440" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stage 0" sheetId="1" r:id="rId1"/>
@@ -907,10 +907,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2467,9 +2467,9 @@
   </sheetPr>
   <dimension ref="A1:AK71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:AJ69"/>
+      <selection pane="bottomLeft" activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2551,33 +2551,33 @@
       <c r="E2" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
       <c r="I2" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="74"/>
+      <c r="J2" s="73"/>
       <c r="K2" s="26" t="s">
         <v>30</v>
       </c>
       <c r="L2" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="74"/>
-      <c r="N2" s="73" t="s">
+      <c r="M2" s="73"/>
+      <c r="N2" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="74"/>
+      <c r="O2" s="73"/>
       <c r="P2" s="18" t="s">
         <v>36</v>
       </c>
       <c r="Q2" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74"/>
+      <c r="T2" s="73"/>
       <c r="U2" s="18" t="s">
         <v>22</v>
       </c>
@@ -2587,27 +2587,27 @@
       <c r="W2" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="73"/>
       <c r="Z2" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="74"/>
+      <c r="AA2" s="73"/>
       <c r="AB2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="AC2" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="73"/>
-      <c r="AE2" s="74"/>
+      <c r="AD2" s="74"/>
+      <c r="AE2" s="73"/>
       <c r="AF2" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="AG2" s="73"/>
-      <c r="AH2" s="73"/>
-      <c r="AI2" s="73"/>
-      <c r="AJ2" s="74"/>
+      <c r="AG2" s="74"/>
+      <c r="AH2" s="74"/>
+      <c r="AI2" s="74"/>
+      <c r="AJ2" s="73"/>
     </row>
     <row r="3" spans="1:37" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="65">
@@ -10251,12 +10251,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="AF71:AJ71"/>
-    <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="A1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E71:H71"/>
@@ -10270,6 +10264,12 @@
     <mergeCell ref="I71:J71"/>
     <mergeCell ref="L71:M71"/>
     <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="AF71:AJ71"/>
+    <mergeCell ref="AF2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11225,8 +11225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AJ65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
RTI + RTS fixed by adding state. ISR working
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="156">
   <si>
     <t>PC</t>
   </si>
@@ -1481,10 +1481,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1499,8 +1499,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1850,7 +1850,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:V19"/>
+      <selection activeCell="B5" sqref="B5:V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2987,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="96">
         <v>1</v>
@@ -3005,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="96">
         <v>0</v>
@@ -3110,6 +3110,74 @@
       </c>
       <c r="V19" s="97">
         <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="95">
+        <v>1</v>
+      </c>
+      <c r="C20" s="96">
+        <v>0</v>
+      </c>
+      <c r="D20" s="97">
+        <v>1</v>
+      </c>
+      <c r="E20" s="96">
+        <v>1</v>
+      </c>
+      <c r="F20" s="97">
+        <v>0</v>
+      </c>
+      <c r="G20" s="96">
+        <v>1</v>
+      </c>
+      <c r="H20" s="97">
+        <v>0</v>
+      </c>
+      <c r="I20" s="96">
+        <v>1</v>
+      </c>
+      <c r="J20" s="97">
+        <v>1</v>
+      </c>
+      <c r="K20" s="96">
+        <v>0</v>
+      </c>
+      <c r="L20" s="97">
+        <v>1</v>
+      </c>
+      <c r="M20" s="97">
+        <v>1</v>
+      </c>
+      <c r="N20" s="95">
+        <v>1</v>
+      </c>
+      <c r="O20" s="96">
+        <v>0</v>
+      </c>
+      <c r="P20" s="97">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="96">
+        <v>1</v>
+      </c>
+      <c r="R20" s="98">
+        <v>1</v>
+      </c>
+      <c r="S20" s="97">
+        <v>1</v>
+      </c>
+      <c r="T20" s="96">
+        <v>1</v>
+      </c>
+      <c r="U20" s="98">
+        <v>1</v>
+      </c>
+      <c r="V20" s="97">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.25">
@@ -3172,44 +3240,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="105"/>
-      <c r="AC1" s="105"/>
-      <c r="AD1" s="105"/>
-      <c r="AE1" s="105"/>
-      <c r="AF1" s="105"/>
-      <c r="AG1" s="105"/>
-      <c r="AH1" s="105"/>
-      <c r="AI1" s="105"/>
-      <c r="AJ1" s="105"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AA1" s="111"/>
+      <c r="AB1" s="111"/>
+      <c r="AC1" s="111"/>
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="111"/>
+      <c r="AF1" s="111"/>
+      <c r="AG1" s="111"/>
+      <c r="AH1" s="111"/>
+      <c r="AI1" s="111"/>
+      <c r="AJ1" s="111"/>
     </row>
     <row r="2" spans="1:37" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
@@ -3221,66 +3289,66 @@
       <c r="D2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="106" t="s">
+      <c r="E2" s="105" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="107"/>
       <c r="G2" s="107"/>
       <c r="H2" s="107"/>
-      <c r="I2" s="106" t="s">
+      <c r="I2" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="111"/>
+      <c r="J2" s="106"/>
       <c r="K2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="106" t="s">
+      <c r="L2" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="111"/>
+      <c r="M2" s="106"/>
       <c r="N2" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="111"/>
+      <c r="O2" s="106"/>
       <c r="P2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="106" t="s">
+      <c r="Q2" s="105" t="s">
         <v>121</v>
       </c>
       <c r="R2" s="107"/>
       <c r="S2" s="107"/>
-      <c r="T2" s="111"/>
+      <c r="T2" s="106"/>
       <c r="U2" s="16" t="s">
         <v>22</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="106" t="s">
+      <c r="W2" s="105" t="s">
         <v>53</v>
       </c>
       <c r="X2" s="107"/>
-      <c r="Y2" s="111"/>
-      <c r="Z2" s="106" t="s">
+      <c r="Y2" s="106"/>
+      <c r="Z2" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="111"/>
+      <c r="AA2" s="106"/>
       <c r="AB2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="106" t="s">
+      <c r="AC2" s="105" t="s">
         <v>58</v>
       </c>
       <c r="AD2" s="107"/>
-      <c r="AE2" s="111"/>
-      <c r="AF2" s="106" t="s">
+      <c r="AE2" s="106"/>
+      <c r="AF2" s="105" t="s">
         <v>46</v>
       </c>
       <c r="AG2" s="107"/>
       <c r="AH2" s="107"/>
       <c r="AI2" s="107"/>
-      <c r="AJ2" s="111"/>
+      <c r="AJ2" s="106"/>
     </row>
     <row r="3" spans="1:37" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="63">
@@ -11700,9 +11768,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="A1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E78:H78"/>
@@ -11719,6 +11784,9 @@
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AF2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11727,10 +11795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W15"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:W15"/>
+      <selection activeCell="C1" sqref="C1:W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12675,7 +12743,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="96">
         <v>1</v>
@@ -12693,7 +12761,7 @@
         <v>1</v>
       </c>
       <c r="K14" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="96">
         <v>0</v>
@@ -12801,6 +12869,77 @@
       </c>
       <c r="W15" s="97">
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="95">
+        <v>1</v>
+      </c>
+      <c r="D16" s="96">
+        <v>0</v>
+      </c>
+      <c r="E16" s="97">
+        <v>1</v>
+      </c>
+      <c r="F16" s="96">
+        <v>1</v>
+      </c>
+      <c r="G16" s="97">
+        <v>0</v>
+      </c>
+      <c r="H16" s="96">
+        <v>1</v>
+      </c>
+      <c r="I16" s="97">
+        <v>0</v>
+      </c>
+      <c r="J16" s="96">
+        <v>1</v>
+      </c>
+      <c r="K16" s="97">
+        <v>1</v>
+      </c>
+      <c r="L16" s="96">
+        <v>0</v>
+      </c>
+      <c r="M16" s="97">
+        <v>1</v>
+      </c>
+      <c r="N16" s="97">
+        <v>1</v>
+      </c>
+      <c r="O16" s="95">
+        <v>1</v>
+      </c>
+      <c r="P16" s="96">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="97">
+        <v>0</v>
+      </c>
+      <c r="R16" s="96">
+        <v>1</v>
+      </c>
+      <c r="S16" s="98">
+        <v>1</v>
+      </c>
+      <c r="T16" s="97">
+        <v>1</v>
+      </c>
+      <c r="U16" s="96">
+        <v>1</v>
+      </c>
+      <c r="V16" s="98">
+        <v>1</v>
+      </c>
+      <c r="W16" s="97">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
about to add CP to ALU
</commit_message>
<xml_diff>
--- a/Documentation/Controller State Table.xlsx
+++ b/Documentation/Controller State Table.xlsx
@@ -1481,10 +1481,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1499,8 +1499,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3014,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="95">
         <v>1</v>
@@ -3150,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="M20" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" s="95">
         <v>1</v>
@@ -3240,44 +3240,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="111"/>
-      <c r="E1" s="111"/>
-      <c r="F1" s="111"/>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-      <c r="M1" s="111"/>
-      <c r="N1" s="111"/>
-      <c r="O1" s="111"/>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="111"/>
-      <c r="S1" s="111"/>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="111"/>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="111"/>
-      <c r="AC1" s="111"/>
-      <c r="AD1" s="111"/>
-      <c r="AE1" s="111"/>
-      <c r="AF1" s="111"/>
-      <c r="AG1" s="111"/>
-      <c r="AH1" s="111"/>
-      <c r="AI1" s="111"/>
-      <c r="AJ1" s="111"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
+      <c r="AA1" s="105"/>
+      <c r="AB1" s="105"/>
+      <c r="AC1" s="105"/>
+      <c r="AD1" s="105"/>
+      <c r="AE1" s="105"/>
+      <c r="AF1" s="105"/>
+      <c r="AG1" s="105"/>
+      <c r="AH1" s="105"/>
+      <c r="AI1" s="105"/>
+      <c r="AJ1" s="105"/>
     </row>
     <row r="2" spans="1:37" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
@@ -3289,66 +3289,66 @@
       <c r="D2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="106" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="107"/>
       <c r="G2" s="107"/>
       <c r="H2" s="107"/>
-      <c r="I2" s="105" t="s">
+      <c r="I2" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="106"/>
+      <c r="J2" s="111"/>
       <c r="K2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="106" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="106"/>
+      <c r="M2" s="111"/>
       <c r="N2" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="106"/>
+      <c r="O2" s="111"/>
       <c r="P2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="105" t="s">
+      <c r="Q2" s="106" t="s">
         <v>121</v>
       </c>
       <c r="R2" s="107"/>
       <c r="S2" s="107"/>
-      <c r="T2" s="106"/>
+      <c r="T2" s="111"/>
       <c r="U2" s="16" t="s">
         <v>22</v>
       </c>
       <c r="V2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="W2" s="105" t="s">
+      <c r="W2" s="106" t="s">
         <v>53</v>
       </c>
       <c r="X2" s="107"/>
-      <c r="Y2" s="106"/>
-      <c r="Z2" s="105" t="s">
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="106"/>
+      <c r="AA2" s="111"/>
       <c r="AB2" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="105" t="s">
+      <c r="AC2" s="106" t="s">
         <v>58</v>
       </c>
       <c r="AD2" s="107"/>
-      <c r="AE2" s="106"/>
-      <c r="AF2" s="105" t="s">
+      <c r="AE2" s="111"/>
+      <c r="AF2" s="106" t="s">
         <v>46</v>
       </c>
       <c r="AG2" s="107"/>
       <c r="AH2" s="107"/>
       <c r="AI2" s="107"/>
-      <c r="AJ2" s="106"/>
+      <c r="AJ2" s="111"/>
     </row>
     <row r="3" spans="1:37" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="63">
@@ -11768,6 +11768,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="AF78:AJ78"/>
+    <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="A1:AJ1"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E78:H78"/>
@@ -11784,9 +11787,6 @@
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AC2:AE2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="AF78:AJ78"/>
-    <mergeCell ref="AF2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="72" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -12770,7 +12770,7 @@
         <v>1</v>
       </c>
       <c r="N14" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="95">
         <v>1</v>
@@ -12912,7 +12912,7 @@
         <v>1</v>
       </c>
       <c r="N16" s="97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O16" s="95">
         <v>1</v>

</xml_diff>